<commit_message>
Work in progress on geocoding functionality
</commit_message>
<xml_diff>
--- a/requirements_sports-event-system-1.xlsx
+++ b/requirements_sports-event-system-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sander Peeters\Desktop\Case Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{41417DF0-6BB2-4841-83A1-05CB506968AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD9C80D1-030A-4660-91BD-19B76052F4CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15750" yWindow="1620" windowWidth="24375" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1965" yWindow="1320" windowWidth="17190" windowHeight="11205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>Req. No.</t>
   </si>
@@ -104,6 +104,12 @@
   </si>
   <si>
     <t>Next</t>
+  </si>
+  <si>
+    <t>Filtering</t>
+  </si>
+  <si>
+    <t>Filtering the results by category, region, etc</t>
   </si>
 </sst>
 </file>
@@ -443,7 +449,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,8 +578,21 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>

</xml_diff>